<commit_message>
almost ready to roll out 1st version but still needs model training for accuracy
</commit_message>
<xml_diff>
--- a/form_responses.xlsx
+++ b/form_responses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Timestamp</t>
   </si>
@@ -56,6 +56,48 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=1oMt24XkiQaIhVMhNwHxS-4oc_KEogwie</t>
+  </si>
+  <si>
+    <t>devanshishukla134@gmail.com</t>
+  </si>
+  <si>
+    <t>Devanshi</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=18PnYHdfpTPWMuPOgsXmnEfu0KFOosY5q</t>
+  </si>
+  <si>
+    <t>2022-26</t>
+  </si>
+  <si>
+    <t>bhatt101.sanjaybhatt@gmail.com</t>
+  </si>
+  <si>
+    <t>Kanishk Bhatt</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1iU5KJ1Mx1M3_8j8xn84vykYac82jwXfA</t>
+  </si>
+  <si>
+    <t>tanusar.40@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saransh Pandey </t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=16YP94hQq5Ab7nnyIaJXjWyYCoUn2PTlp</t>
+  </si>
+  <si>
+    <t>aadityap0320@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aaditya Pandey </t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1b865zBX4AoFnkg5fXOhkzdo8xBmk6Eyu</t>
   </si>
 </sst>
 </file>
@@ -65,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -87,6 +129,21 @@
       <color rgb="FF434343"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -96,7 +153,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border/>
     <border>
       <left style="thin">
@@ -180,6 +237,48 @@
       </top>
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
       </bottom>
     </border>
     <border>
@@ -228,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -263,6 +362,33 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -323,7 +449,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G3" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G7" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="7">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -618,14 +744,110 @@
         <v>2022.0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="12">
+        <v>45898.97728313657</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="13">
+        <v>58976.0</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8">
+        <v>45925.73636170139</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="9">
+        <v>59251.0</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="11">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12">
+        <v>45925.750126087965</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="13">
+        <v>58857.0</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="15">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="17">
+        <v>45925.75735321759</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="18">
+        <v>58863.0</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="20">
+        <v>2022.0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2"/>
     <hyperlink r:id="rId2" ref="F3"/>
+    <hyperlink r:id="rId3" ref="F4"/>
+    <hyperlink r:id="rId4" ref="F5"/>
+    <hyperlink r:id="rId5" ref="F6"/>
+    <hyperlink r:id="rId6" ref="F7"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>